<commit_message>
Revised with code changes
</commit_message>
<xml_diff>
--- a/samples/BulbData.xlsx
+++ b/samples/BulbData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omniverse\PlaybookOV\playbook-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omniverse\PlaybookOV\playbook-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D066D4-5DDF-4307-A001-2D20588CCBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC79299A-FB4F-49B0-B986-EFCB1860A549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26808" yWindow="4176" windowWidth="13632" windowHeight="11196" xr2:uid="{C208CA14-DB58-4184-8A4B-47C982339907}"/>
   </bookViews>
@@ -87,7 +87,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,13 +101,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -122,13 +136,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -145,7 +170,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A53B95E-BD6B-4DA7-B42A-71A9144A704A}" name="Table1" displayName="Table1" ref="B2:F7" totalsRowShown="0">
   <autoFilter ref="B2:F7" xr:uid="{9A53B95E-BD6B-4DA7-B42A-71A9144A704A}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D5FD6D7B-9371-48D5-89AF-A6EA710EF597}" name="Name"/>
+    <tableColumn id="1" xr3:uid="{D5FD6D7B-9371-48D5-89AF-A6EA710EF597}" name="Name" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{47AD99A6-4460-4D54-B52F-1986ECAEBEB0}" name="Prim Path"/>
     <tableColumn id="3" xr3:uid="{0E9D98EC-2708-4177-ADDD-223C3DE843E4}" name="X Position"/>
     <tableColumn id="4" xr3:uid="{F48BC640-41CF-4A2F-9872-29FD5AF1D7F9}" name="Y Position"/>
@@ -455,16 +480,16 @@
   <dimension ref="B2:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F3" sqref="F3:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" customWidth="1"/>
     <col min="5" max="5" width="6.6640625" customWidth="1"/>
-    <col min="6" max="6" width="5.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
@@ -485,7 +510,7 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
@@ -497,12 +522,12 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3">
-        <v>20</v>
+      <c r="F3" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
@@ -514,12 +539,12 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
-        <v>50</v>
+      <c r="F4" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
@@ -531,12 +556,12 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5">
-        <v>100</v>
+      <c r="F5" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
@@ -548,16 +573,22 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
-        <v>30</v>
+      <c r="F6" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="D7" s="1">
+        <v>-50</v>
+      </c>
+      <c r="E7" s="1">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>